<commit_message>
OE-9291 - display grouping on settings page
</commit_message>
<xml_diff>
--- a/protected/migrations/data/m221109_114900_add_description_grouping_to_settings/setting_metadata_202208211803.xlsx
+++ b/protected/migrations/data/m221109_114900_add_description_grouping_to_settings/setting_metadata_202208211803.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="541">
   <si>
     <t>key</t>
   </si>
@@ -1553,7 +1553,7 @@
     <t>auto_add_book_apt_step</t>
   </si>
   <si>
-    <t>Adds a "Book Appointment" step on follow-up</t>
+    <t>Add a "Book Appointment" step on follow-up</t>
   </si>
   <si>
     <t>The default adds a "book appointment" step to the end of current worklist when a follow up appointment is requested in the examination-&gt;follow-up element for the cataract  (deprecated)</t>
@@ -1607,10 +1607,31 @@
     <t>When On, users must sign CVI events using their PINl. When Off, CVI events will be automatically signed for the current user on save</t>
   </si>
   <si>
+    <t>close_incomplete_exam_elements</t>
+  </si>
+  <si>
+    <t>Offer to automatically close incomplete examination elements</t>
+  </si>
+  <si>
+    <t>When On, if a user has non-mandatory elements open in an examination event AND they have not entered any data into some elements, then upon save a dialog box will show asking if they would like to close (i.e. discard) the empty elements</t>
+  </si>
+  <si>
+    <t>enable_imagenet_integration</t>
+  </si>
+  <si>
+    <t>ImageNET: enable integration</t>
+  </si>
+  <si>
+    <t>Enables or disables the integration to Topcon ImageNET 6 - this integration provides a contextual link to ImageNET for the current OpenEyes patient</t>
+  </si>
+  <si>
     <t>break_glass_patient_institution_field</t>
   </si>
   <si>
     <t>Field for break-glass patient institution</t>
+  </si>
+  <si>
+    <t>If using the Break Glass feature, this setting toggles between the old behaviour - where the County field of the patient's address was used to determine the owning institution - and the new behaviour, which uses a dedicated Primary Institution field. If unsure, use Primary Institution</t>
   </si>
   <si>
     <t>eclo_email</t>
@@ -1966,7 +1987,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E175"/>
+  <dimension ref="A1:E177"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1979,7 +2000,7 @@
     <col min="5" max="5" style="2" width="88.7192857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" hidden="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1996,7 +2017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" hidden="1">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2013,7 +2034,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" hidden="1">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2030,7 +2051,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" hidden="1">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2047,7 +2068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" hidden="1">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -2064,7 +2085,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" hidden="1">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2081,7 +2102,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" hidden="1">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -2098,7 +2119,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" hidden="1">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2115,7 +2136,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" hidden="1">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -2132,7 +2153,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" hidden="1">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -2149,7 +2170,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" hidden="1">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -2166,7 +2187,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" hidden="1">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -2183,7 +2204,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" hidden="1">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -2200,7 +2221,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" hidden="1">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -2217,7 +2238,7 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" hidden="1">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -2232,7 +2253,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" hidden="1">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
@@ -2247,7 +2268,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" hidden="1">
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
@@ -2262,7 +2283,7 @@
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" hidden="1">
       <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
@@ -2277,7 +2298,7 @@
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" hidden="1">
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
@@ -2292,7 +2313,7 @@
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" hidden="1">
       <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
@@ -2307,7 +2328,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" hidden="1">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
@@ -2322,7 +2343,7 @@
         <v>68</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5" hidden="1">
       <c r="A22" s="1" t="s">
         <v>69</v>
       </c>
@@ -2337,7 +2358,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5" hidden="1">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -2354,7 +2375,7 @@
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5" hidden="1">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
@@ -2369,7 +2390,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5" hidden="1">
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
@@ -2384,7 +2405,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5" hidden="1">
       <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
@@ -2399,7 +2420,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" hidden="1">
       <c r="A27" s="1" t="s">
         <v>88</v>
       </c>
@@ -2414,7 +2435,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5" hidden="1">
       <c r="A28" s="1" t="s">
         <v>91</v>
       </c>
@@ -2429,7 +2450,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5" hidden="1">
       <c r="A29" s="1" t="s">
         <v>94</v>
       </c>
@@ -2444,7 +2465,7 @@
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5" hidden="1">
       <c r="A30" s="1" t="s">
         <v>97</v>
       </c>
@@ -2459,7 +2480,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5" hidden="1">
       <c r="A31" s="1" t="s">
         <v>101</v>
       </c>
@@ -2474,7 +2495,7 @@
         <v>103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5" hidden="1">
       <c r="A32" s="1" t="s">
         <v>104</v>
       </c>
@@ -2489,7 +2510,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5" hidden="1">
       <c r="A33" s="1" t="s">
         <v>108</v>
       </c>
@@ -2504,7 +2525,7 @@
         <v>110</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5" hidden="1">
       <c r="A34" s="1" t="s">
         <v>111</v>
       </c>
@@ -2519,7 +2540,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5" hidden="1">
       <c r="A35" s="1" t="s">
         <v>114</v>
       </c>
@@ -2534,7 +2555,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5" hidden="1">
       <c r="A36" s="1" t="s">
         <v>117</v>
       </c>
@@ -2549,7 +2570,7 @@
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5" hidden="1">
       <c r="A37" s="1" t="s">
         <v>120</v>
       </c>
@@ -2564,7 +2585,7 @@
         <v>122</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5" hidden="1">
       <c r="A38" s="1" t="s">
         <v>123</v>
       </c>
@@ -2579,7 +2600,7 @@
         <v>125</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5" hidden="1">
       <c r="A39" s="1" t="s">
         <v>126</v>
       </c>
@@ -2594,7 +2615,7 @@
         <v>128</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5" hidden="1">
       <c r="A40" s="1" t="s">
         <v>129</v>
       </c>
@@ -2609,7 +2630,7 @@
         <v>131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5" hidden="1">
       <c r="A41" s="1" t="s">
         <v>132</v>
       </c>
@@ -2624,7 +2645,7 @@
         <v>134</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5" hidden="1">
       <c r="A42" s="1" t="s">
         <v>135</v>
       </c>
@@ -2639,7 +2660,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5" hidden="1">
       <c r="A43" s="1" t="s">
         <v>138</v>
       </c>
@@ -2654,7 +2675,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5" hidden="1">
       <c r="A44" s="1" t="s">
         <v>141</v>
       </c>
@@ -2669,7 +2690,7 @@
         <v>143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5" hidden="1">
       <c r="A45" s="1" t="s">
         <v>144</v>
       </c>
@@ -2684,7 +2705,7 @@
         <v>146</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5" hidden="1">
       <c r="A46" s="1" t="s">
         <v>147</v>
       </c>
@@ -2699,7 +2720,7 @@
         <v>149</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5" hidden="1">
       <c r="A47" s="1" t="s">
         <v>150</v>
       </c>
@@ -2714,7 +2735,7 @@
         <v>152</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5" hidden="1">
       <c r="A48" s="1" t="s">
         <v>153</v>
       </c>
@@ -2729,7 +2750,7 @@
         <v>155</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5" hidden="1">
       <c r="A49" s="1" t="s">
         <v>156</v>
       </c>
@@ -2744,7 +2765,7 @@
         <v>158</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5" hidden="1">
       <c r="A50" s="1" t="s">
         <v>159</v>
       </c>
@@ -2759,7 +2780,7 @@
         <v>161</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5" hidden="1">
       <c r="A51" s="1" t="s">
         <v>162</v>
       </c>
@@ -2774,7 +2795,7 @@
         <v>164</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5" hidden="1">
       <c r="A52" s="1" t="s">
         <v>165</v>
       </c>
@@ -2789,7 +2810,7 @@
         <v>167</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5" hidden="1">
       <c r="A53" s="1" t="s">
         <v>168</v>
       </c>
@@ -2804,7 +2825,7 @@
         <v>170</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5" hidden="1">
       <c r="A54" s="1" t="s">
         <v>171</v>
       </c>
@@ -2819,7 +2840,7 @@
         <v>173</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5" hidden="1">
       <c r="A55" s="1" t="s">
         <v>174</v>
       </c>
@@ -2834,7 +2855,7 @@
         <v>176</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5" hidden="1">
       <c r="A56" s="1" t="s">
         <v>177</v>
       </c>
@@ -2849,7 +2870,7 @@
         <v>179</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5" hidden="1">
       <c r="A57" s="1" t="s">
         <v>180</v>
       </c>
@@ -2864,7 +2885,7 @@
         <v>182</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5" hidden="1">
       <c r="A58" s="1" t="s">
         <v>183</v>
       </c>
@@ -2879,7 +2900,7 @@
         <v>185</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5" hidden="1">
       <c r="A59" s="1" t="s">
         <v>186</v>
       </c>
@@ -2894,7 +2915,7 @@
         <v>188</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5" hidden="1">
       <c r="A60" s="1" t="s">
         <v>189</v>
       </c>
@@ -2909,7 +2930,7 @@
         <v>191</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5" hidden="1">
       <c r="A61" s="1" t="s">
         <v>192</v>
       </c>
@@ -2924,7 +2945,7 @@
         <v>194</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5" hidden="1">
       <c r="A62" s="1" t="s">
         <v>195</v>
       </c>
@@ -2939,7 +2960,7 @@
         <v>198</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5" hidden="1">
       <c r="A63" s="1" t="s">
         <v>199</v>
       </c>
@@ -2954,7 +2975,7 @@
         <v>201</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5" hidden="1">
       <c r="A64" s="1" t="s">
         <v>202</v>
       </c>
@@ -2969,7 +2990,7 @@
         <v>204</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5" hidden="1">
       <c r="A65" s="1" t="s">
         <v>205</v>
       </c>
@@ -2984,7 +3005,7 @@
         <v>208</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5" hidden="1">
       <c r="A66" s="1" t="s">
         <v>209</v>
       </c>
@@ -2999,7 +3020,7 @@
         <v>211</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5" hidden="1">
       <c r="A67" s="1" t="s">
         <v>212</v>
       </c>
@@ -3014,7 +3035,7 @@
         <v>214</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5" hidden="1">
       <c r="A68" s="1" t="s">
         <v>215</v>
       </c>
@@ -3029,7 +3050,7 @@
         <v>217</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5" hidden="1">
       <c r="A69" s="1" t="s">
         <v>218</v>
       </c>
@@ -3044,7 +3065,7 @@
         <v>220</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5" hidden="1">
       <c r="A70" s="1" t="s">
         <v>221</v>
       </c>
@@ -3059,7 +3080,7 @@
         <v>223</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5" hidden="1">
       <c r="A71" s="1" t="s">
         <v>224</v>
       </c>
@@ -3074,7 +3095,7 @@
         <v>226</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5" hidden="1">
       <c r="A72" s="1" t="s">
         <v>227</v>
       </c>
@@ -3089,7 +3110,7 @@
         <v>229</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5" hidden="1">
       <c r="A73" s="1" t="s">
         <v>230</v>
       </c>
@@ -3104,7 +3125,7 @@
         <v>232</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5" hidden="1">
       <c r="A74" s="1" t="s">
         <v>233</v>
       </c>
@@ -3119,7 +3140,7 @@
         <v>235</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5" hidden="1">
       <c r="A75" s="1" t="s">
         <v>236</v>
       </c>
@@ -3134,7 +3155,7 @@
         <v>238</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5" hidden="1">
       <c r="A76" s="1" t="s">
         <v>239</v>
       </c>
@@ -3149,7 +3170,7 @@
         <v>241</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5" hidden="1">
       <c r="A77" s="1" t="s">
         <v>242</v>
       </c>
@@ -3164,7 +3185,7 @@
         <v>244</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5" hidden="1">
       <c r="A78" s="1" t="s">
         <v>245</v>
       </c>
@@ -3179,7 +3200,7 @@
         <v>247</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5" hidden="1">
       <c r="A79" s="1" t="s">
         <v>248</v>
       </c>
@@ -3194,7 +3215,7 @@
         <v>250</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5" hidden="1">
       <c r="A80" s="1" t="s">
         <v>251</v>
       </c>
@@ -3209,7 +3230,7 @@
         <v>253</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5" hidden="1">
       <c r="A81" s="1" t="s">
         <v>254</v>
       </c>
@@ -3224,7 +3245,7 @@
         <v>256</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5" hidden="1">
       <c r="A82" s="1" t="s">
         <v>257</v>
       </c>
@@ -3239,7 +3260,7 @@
         <v>259</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5" hidden="1">
       <c r="A83" s="1" t="s">
         <v>260</v>
       </c>
@@ -3254,7 +3275,7 @@
         <v>262</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5" hidden="1">
       <c r="A84" s="1" t="s">
         <v>263</v>
       </c>
@@ -3269,7 +3290,7 @@
         <v>265</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5" hidden="1">
       <c r="A85" s="1" t="s">
         <v>266</v>
       </c>
@@ -3284,7 +3305,7 @@
         <v>268</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5" hidden="1">
       <c r="A86" s="1" t="s">
         <v>269</v>
       </c>
@@ -3299,7 +3320,7 @@
         <v>271</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5" hidden="1">
       <c r="A87" s="1" t="s">
         <v>272</v>
       </c>
@@ -3314,7 +3335,7 @@
         <v>274</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5" hidden="1">
       <c r="A88" s="1" t="s">
         <v>275</v>
       </c>
@@ -3329,7 +3350,7 @@
         <v>277</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5" hidden="1">
       <c r="A89" s="1" t="s">
         <v>278</v>
       </c>
@@ -3344,7 +3365,7 @@
         <v>280</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5" hidden="1">
       <c r="A90" s="1" t="s">
         <v>281</v>
       </c>
@@ -3359,7 +3380,7 @@
         <v>283</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5" hidden="1">
       <c r="A91" s="1" t="s">
         <v>284</v>
       </c>
@@ -3374,7 +3395,7 @@
         <v>286</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5" hidden="1">
       <c r="A92" s="1" t="s">
         <v>287</v>
       </c>
@@ -3389,7 +3410,7 @@
         <v>289</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5" hidden="1">
       <c r="A93" s="1" t="s">
         <v>290</v>
       </c>
@@ -3404,7 +3425,7 @@
         <v>292</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5" hidden="1">
       <c r="A94" s="1" t="s">
         <v>293</v>
       </c>
@@ -3419,7 +3440,7 @@
         <v>295</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5" hidden="1">
       <c r="A95" s="1" t="s">
         <v>296</v>
       </c>
@@ -3434,7 +3455,7 @@
         <v>298</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5" hidden="1">
       <c r="A96" s="1" t="s">
         <v>299</v>
       </c>
@@ -3449,7 +3470,7 @@
         <v>301</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5" hidden="1">
       <c r="A97" s="1" t="s">
         <v>302</v>
       </c>
@@ -3464,7 +3485,7 @@
         <v>304</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5" hidden="1">
       <c r="A98" s="1" t="s">
         <v>305</v>
       </c>
@@ -3479,7 +3500,7 @@
         <v>307</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5" hidden="1">
       <c r="A99" s="1" t="s">
         <v>308</v>
       </c>
@@ -3494,7 +3515,7 @@
         <v>310</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5" hidden="1">
       <c r="A100" s="1" t="s">
         <v>311</v>
       </c>
@@ -3509,7 +3530,7 @@
         <v>313</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5" hidden="1">
       <c r="A101" s="1" t="s">
         <v>314</v>
       </c>
@@ -3524,7 +3545,7 @@
         <v>316</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5" hidden="1">
       <c r="A102" s="1" t="s">
         <v>317</v>
       </c>
@@ -3541,7 +3562,7 @@
         <v>319</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5" hidden="1">
       <c r="A103" s="1" t="s">
         <v>317</v>
       </c>
@@ -3558,7 +3579,7 @@
         <v>320</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5" hidden="1">
       <c r="A104" s="1" t="s">
         <v>321</v>
       </c>
@@ -3575,7 +3596,7 @@
         <v>324</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5" hidden="1">
       <c r="A105" s="1" t="s">
         <v>325</v>
       </c>
@@ -3592,7 +3613,7 @@
         <v>327</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5" hidden="1">
       <c r="A106" s="1" t="s">
         <v>328</v>
       </c>
@@ -3609,7 +3630,7 @@
         <v>330</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="19.5" hidden="1">
       <c r="A107" s="1" t="s">
         <v>331</v>
       </c>
@@ -3626,7 +3647,7 @@
         <v>333</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="19.5" hidden="1">
       <c r="A108" s="1" t="s">
         <v>334</v>
       </c>
@@ -3643,7 +3664,7 @@
         <v>336</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="19.5" hidden="1">
       <c r="A109" s="1" t="s">
         <v>337</v>
       </c>
@@ -3660,7 +3681,7 @@
         <v>340</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="19.5" hidden="1">
       <c r="A110" s="1" t="s">
         <v>341</v>
       </c>
@@ -3677,7 +3698,7 @@
         <v>343</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="19.5" hidden="1">
       <c r="A111" s="1" t="s">
         <v>344</v>
       </c>
@@ -3694,7 +3715,7 @@
         <v>346</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="19.5" hidden="1">
       <c r="A112" s="1" t="s">
         <v>347</v>
       </c>
@@ -3711,7 +3732,7 @@
         <v>349</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="19.5" hidden="1">
       <c r="A113" s="1" t="s">
         <v>350</v>
       </c>
@@ -3728,7 +3749,7 @@
         <v>352</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="19.5" hidden="1">
       <c r="A114" s="1" t="s">
         <v>353</v>
       </c>
@@ -3745,7 +3766,7 @@
         <v>355</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="19.5" hidden="1">
       <c r="A115" s="1" t="s">
         <v>356</v>
       </c>
@@ -3760,7 +3781,7 @@
         <v>358</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="19.5" hidden="1">
       <c r="A116" s="1" t="s">
         <v>359</v>
       </c>
@@ -3775,7 +3796,7 @@
         <v>361</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="19.5" hidden="1">
       <c r="A117" s="1" t="s">
         <v>362</v>
       </c>
@@ -3790,7 +3811,7 @@
         <v>364</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="19.5" hidden="1">
       <c r="A118" s="1" t="s">
         <v>365</v>
       </c>
@@ -3805,7 +3826,7 @@
         <v>367</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="19.5" hidden="1">
       <c r="A119" s="1" t="s">
         <v>368</v>
       </c>
@@ -3820,7 +3841,7 @@
         <v>370</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="19.5" hidden="1">
       <c r="A120" s="1" t="s">
         <v>371</v>
       </c>
@@ -3835,7 +3856,7 @@
         <v>373</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="19.5" hidden="1">
       <c r="A121" s="1" t="s">
         <v>374</v>
       </c>
@@ -3850,7 +3871,7 @@
         <v>376</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="19.5" hidden="1">
       <c r="A122" s="1" t="s">
         <v>377</v>
       </c>
@@ -3865,7 +3886,7 @@
         <v>379</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="19.5" hidden="1">
       <c r="A123" s="1" t="s">
         <v>380</v>
       </c>
@@ -3880,7 +3901,7 @@
         <v>382</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="19.5" hidden="1">
       <c r="A124" s="1" t="s">
         <v>383</v>
       </c>
@@ -3895,7 +3916,7 @@
         <v>385</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="19.5" hidden="1">
       <c r="A125" s="1" t="s">
         <v>386</v>
       </c>
@@ -3910,7 +3931,7 @@
         <v>388</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="19.5" hidden="1">
       <c r="A126" s="1" t="s">
         <v>389</v>
       </c>
@@ -3925,7 +3946,7 @@
         <v>391</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="19.5" hidden="1">
       <c r="A127" s="1" t="s">
         <v>392</v>
       </c>
@@ -3940,7 +3961,7 @@
         <v>394</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="19.5" hidden="1">
       <c r="A128" s="1" t="s">
         <v>395</v>
       </c>
@@ -3955,7 +3976,7 @@
         <v>398</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="19.5" hidden="1">
       <c r="A129" s="1" t="s">
         <v>399</v>
       </c>
@@ -3970,7 +3991,7 @@
         <v>402</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="19.5" hidden="1">
       <c r="A130" s="1" t="s">
         <v>403</v>
       </c>
@@ -3985,7 +4006,7 @@
         <v>405</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="19.5" hidden="1">
       <c r="A131" s="1" t="s">
         <v>406</v>
       </c>
@@ -4000,7 +4021,7 @@
         <v>408</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="19.5" hidden="1">
       <c r="A132" s="1" t="s">
         <v>409</v>
       </c>
@@ -4015,7 +4036,7 @@
         <v>408</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="19.5" hidden="1">
       <c r="A133" s="1" t="s">
         <v>411</v>
       </c>
@@ -4030,7 +4051,7 @@
         <v>408</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="19.5" hidden="1">
       <c r="A134" s="1" t="s">
         <v>413</v>
       </c>
@@ -4045,7 +4066,7 @@
         <v>408</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="19.5" hidden="1">
       <c r="A135" s="1" t="s">
         <v>415</v>
       </c>
@@ -4060,7 +4081,7 @@
         <v>417</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="19.5" hidden="1">
       <c r="A136" s="1" t="s">
         <v>418</v>
       </c>
@@ -4075,7 +4096,7 @@
         <v>420</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="19.5" hidden="1">
       <c r="A137" s="1" t="s">
         <v>421</v>
       </c>
@@ -4090,7 +4111,7 @@
         <v>420</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="19.5" hidden="1">
       <c r="A138" s="1" t="s">
         <v>423</v>
       </c>
@@ -4105,7 +4126,7 @@
         <v>420</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="19.5" hidden="1">
       <c r="A139" s="1" t="s">
         <v>425</v>
       </c>
@@ -4120,7 +4141,7 @@
         <v>420</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="19.5" hidden="1">
       <c r="A140" s="1" t="s">
         <v>427</v>
       </c>
@@ -4135,7 +4156,7 @@
         <v>429</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="19.5" hidden="1">
       <c r="A141" s="1" t="s">
         <v>430</v>
       </c>
@@ -4150,7 +4171,7 @@
         <v>432</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="19.5" hidden="1">
       <c r="A142" s="1" t="s">
         <v>433</v>
       </c>
@@ -4165,7 +4186,7 @@
         <v>435</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="19.5" hidden="1">
       <c r="A143" s="1" t="s">
         <v>436</v>
       </c>
@@ -4180,7 +4201,7 @@
         <v>438</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="19.5" hidden="1">
       <c r="A144" s="1" t="s">
         <v>439</v>
       </c>
@@ -4195,7 +4216,7 @@
         <v>441</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="19.5" hidden="1">
       <c r="A145" s="1" t="s">
         <v>442</v>
       </c>
@@ -4210,7 +4231,7 @@
         <v>444</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="19.5" hidden="1">
       <c r="A146" s="1" t="s">
         <v>445</v>
       </c>
@@ -4225,7 +4246,7 @@
         <v>447</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="19.5" hidden="1">
       <c r="A147" s="1" t="s">
         <v>448</v>
       </c>
@@ -4240,7 +4261,7 @@
         <v>450</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="19.5" hidden="1">
       <c r="A148" s="1" t="s">
         <v>451</v>
       </c>
@@ -4255,7 +4276,7 @@
         <v>453</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="19.5" hidden="1">
       <c r="A149" s="1" t="s">
         <v>454</v>
       </c>
@@ -4270,7 +4291,7 @@
         <v>456</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="19.5" hidden="1">
       <c r="A150" s="1" t="s">
         <v>457</v>
       </c>
@@ -4285,7 +4306,7 @@
         <v>460</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="19.5" hidden="1">
       <c r="A151" s="1" t="s">
         <v>461</v>
       </c>
@@ -4300,7 +4321,7 @@
         <v>463</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="19.5" hidden="1">
       <c r="A152" s="1" t="s">
         <v>464</v>
       </c>
@@ -4315,7 +4336,7 @@
         <v>466</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="19.5" hidden="1">
       <c r="A153" s="1" t="s">
         <v>467</v>
       </c>
@@ -4330,7 +4351,7 @@
         <v>470</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="19.5" hidden="1">
       <c r="A154" s="1" t="s">
         <v>471</v>
       </c>
@@ -4345,7 +4366,7 @@
         <v>470</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="19.5" hidden="1">
       <c r="A155" s="1" t="s">
         <v>473</v>
       </c>
@@ -4360,7 +4381,7 @@
         <v>475</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="19.5" hidden="1">
       <c r="A156" s="1" t="s">
         <v>476</v>
       </c>
@@ -4375,7 +4396,7 @@
         <v>478</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="19.5" hidden="1">
       <c r="A157" s="1" t="s">
         <v>479</v>
       </c>
@@ -4390,7 +4411,7 @@
         <v>470</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="19.5" hidden="1">
       <c r="A158" s="1" t="s">
         <v>481</v>
       </c>
@@ -4405,7 +4426,7 @@
         <v>470</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="19.5" hidden="1">
       <c r="A159" s="1" t="s">
         <v>483</v>
       </c>
@@ -4420,7 +4441,7 @@
         <v>485</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5" hidden="1">
       <c r="A160" s="1" t="s">
         <v>486</v>
       </c>
@@ -4435,7 +4456,7 @@
         <v>488</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="19.5" hidden="1">
       <c r="A161" s="1" t="s">
         <v>489</v>
       </c>
@@ -4450,7 +4471,7 @@
         <v>491</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="19.5" hidden="1">
       <c r="A162" s="1" t="s">
         <v>492</v>
       </c>
@@ -4465,7 +4486,7 @@
         <v>494</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="19.5" hidden="1">
       <c r="A163" s="1" t="s">
         <v>495</v>
       </c>
@@ -4480,7 +4501,7 @@
         <v>497</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="19.5" hidden="1">
       <c r="A164" s="1" t="s">
         <v>498</v>
       </c>
@@ -4495,7 +4516,7 @@
         <v>500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="19.5" hidden="1">
       <c r="A165" s="1" t="s">
         <v>501</v>
       </c>
@@ -4510,7 +4531,7 @@
         <v>503</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="19.5" hidden="1">
       <c r="A166" s="1" t="s">
         <v>504</v>
       </c>
@@ -4525,7 +4546,7 @@
         <v>506</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="19.5" hidden="1">
       <c r="A167" s="1" t="s">
         <v>507</v>
       </c>
@@ -4555,7 +4576,7 @@
         <v>512</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="19.5" hidden="1">
       <c r="A169" s="1" t="s">
         <v>513</v>
       </c>
@@ -4570,7 +4591,7 @@
         <v>515</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="19.5" hidden="1">
       <c r="A170" s="1" t="s">
         <v>516</v>
       </c>
@@ -4585,7 +4606,7 @@
         <v>518</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="19.5" hidden="1">
       <c r="A171" s="1" t="s">
         <v>519</v>
       </c>
@@ -4600,7 +4621,7 @@
         <v>521</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="19.5" hidden="1">
       <c r="A172" s="1" t="s">
         <v>522</v>
       </c>
@@ -4615,7 +4636,7 @@
         <v>525</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="19.5" hidden="1">
       <c r="A173" s="1" t="s">
         <v>526</v>
       </c>
@@ -4630,7 +4651,7 @@
         <v>528</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="19.5" hidden="1">
       <c r="A174" s="1" t="s">
         <v>529</v>
       </c>
@@ -4639,23 +4660,55 @@
         <v>530</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E174" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="19.5">
+        <v>13</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="19.5" hidden="1">
       <c r="A175" s="1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B175" s="1"/>
       <c r="C175" s="1" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D175" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="19.5" hidden="1">
+      <c r="A176" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="19.5" hidden="1">
+      <c r="A177" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B177" s="1"/>
+      <c r="C177" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="D177" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="E175" s="1" t="s">
-        <v>533</v>
+      <c r="E177" s="1" t="s">
+        <v>540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OE-9291 - more settings and don't show empty groups
</commit_message>
<xml_diff>
--- a/protected/migrations/data/m221109_114900_add_description_grouping_to_settings/setting_metadata_202208211803.xlsx
+++ b/protected/migrations/data/m221109_114900_add_description_grouping_to_settings/setting_metadata_202208211803.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="541">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="553">
   <si>
     <t>key</t>
   </si>
@@ -1433,6 +1433,15 @@
     <t>Does not appear to be used. Delete? This should be using the default SMTP sender details</t>
   </si>
   <si>
+    <t>cvi_la_delivery_enabled</t>
+  </si>
+  <si>
+    <t>CVI delivery enable to send to LA</t>
+  </si>
+  <si>
+    <t>Turn this On to enable electronic delivery of CVI applications to the Local Authority</t>
+  </si>
+  <si>
     <t>cvidelivery_la_sender_name</t>
   </si>
   <si>
@@ -1496,6 +1505,15 @@
     <t>The body text for emails sent to RCOph for Certificate of Visual Impairment applications. Note that the actual application is attached to the email as a PDF</t>
   </si>
   <si>
+    <t>cvi_rcop_delivery_enabled</t>
+  </si>
+  <si>
+    <t>CVI delivery enable to send to RCOP</t>
+  </si>
+  <si>
+    <t>Turn this On to enable electronic delivery of CVI applications to the Royal College of Ophthalmologists</t>
+  </si>
+  <si>
     <t>cvi_eclo_target_email</t>
   </si>
   <si>
@@ -1505,13 +1523,31 @@
     <t>The email address to send CVI Applications to for the ECLO team</t>
   </si>
   <si>
+    <t>cvi_eclo_notification_email</t>
+  </si>
+  <si>
+    <t>CVI Delivery to ECLO</t>
+  </si>
+  <si>
+    <t>Turn this On to enable electronic delivery of CVI applications to the Eye Care Liason Officer</t>
+  </si>
+  <si>
     <t>cvi_eclo_sender_email</t>
   </si>
   <si>
     <t>Sender address for ECLO notifications</t>
   </si>
   <si>
-    <t>The email address to send CVI Applications from for the ECLO team</t>
+    <t>The email address to send CVI Applications from for the Eye Care Liason Office team</t>
+  </si>
+  <si>
+    <t>cvi_docman_delivery_enabled</t>
+  </si>
+  <si>
+    <t>CVI delivery enable to send to GP</t>
+  </si>
+  <si>
+    <t>Turn this On to enable electronic delivery of CVI applications to the patient's GP</t>
   </si>
   <si>
     <t>dob_mandatory_in_search</t>
@@ -1987,20 +2023,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E177"/>
+  <dimension ref="A1:E181"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="51.14785714285715" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="2" width="57.29071428571429" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="2" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="88.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="2" width="203.29071428571427" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2017,7 +2053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2034,7 +2070,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2051,7 +2087,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -2068,7 +2104,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -2085,7 +2121,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -2102,7 +2138,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -2119,7 +2155,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -2136,7 +2172,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -2153,7 +2189,7 @@
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -2170,7 +2206,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -2187,7 +2223,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -2204,7 +2240,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -2221,7 +2257,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -2238,7 +2274,7 @@
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -2253,7 +2289,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
         <v>51</v>
       </c>
@@ -2268,7 +2304,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
         <v>54</v>
       </c>
@@ -2283,7 +2319,7 @@
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
         <v>57</v>
       </c>
@@ -2298,7 +2334,7 @@
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
         <v>60</v>
       </c>
@@ -2313,7 +2349,7 @@
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
@@ -2328,7 +2364,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
@@ -2343,7 +2379,7 @@
         <v>68</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
         <v>69</v>
       </c>
@@ -2358,7 +2394,7 @@
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
         <v>10</v>
       </c>
@@ -2375,7 +2411,7 @@
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
@@ -2390,7 +2426,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
@@ -2405,7 +2441,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
@@ -2420,7 +2456,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1" t="s">
         <v>88</v>
       </c>
@@ -2435,7 +2471,7 @@
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1" t="s">
         <v>91</v>
       </c>
@@ -2450,7 +2486,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="1" t="s">
         <v>94</v>
       </c>
@@ -2465,7 +2501,7 @@
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1" t="s">
         <v>97</v>
       </c>
@@ -2480,7 +2516,7 @@
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="1" t="s">
         <v>101</v>
       </c>
@@ -2495,7 +2531,7 @@
         <v>103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="1" t="s">
         <v>104</v>
       </c>
@@ -2510,7 +2546,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="1" t="s">
         <v>108</v>
       </c>
@@ -2525,7 +2561,7 @@
         <v>110</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="1" t="s">
         <v>111</v>
       </c>
@@ -2540,7 +2576,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="1" t="s">
         <v>114</v>
       </c>
@@ -2555,7 +2591,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="1" t="s">
         <v>117</v>
       </c>
@@ -2570,7 +2606,7 @@
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="1" t="s">
         <v>120</v>
       </c>
@@ -2585,7 +2621,7 @@
         <v>122</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1" t="s">
         <v>123</v>
       </c>
@@ -2600,7 +2636,7 @@
         <v>125</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="1" t="s">
         <v>126</v>
       </c>
@@ -2615,7 +2651,7 @@
         <v>128</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="1" t="s">
         <v>129</v>
       </c>
@@ -2630,7 +2666,7 @@
         <v>131</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="1" t="s">
         <v>132</v>
       </c>
@@ -2645,7 +2681,7 @@
         <v>134</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="1" t="s">
         <v>135</v>
       </c>
@@ -2660,7 +2696,7 @@
         <v>137</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1" t="s">
         <v>138</v>
       </c>
@@ -2675,7 +2711,7 @@
         <v>140</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1" t="s">
         <v>141</v>
       </c>
@@ -2690,7 +2726,7 @@
         <v>143</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1" t="s">
         <v>144</v>
       </c>
@@ -2705,7 +2741,7 @@
         <v>146</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1" t="s">
         <v>147</v>
       </c>
@@ -2720,7 +2756,7 @@
         <v>149</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1" t="s">
         <v>150</v>
       </c>
@@ -2735,7 +2771,7 @@
         <v>152</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1" t="s">
         <v>153</v>
       </c>
@@ -2750,7 +2786,7 @@
         <v>155</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="1" t="s">
         <v>156</v>
       </c>
@@ -2765,7 +2801,7 @@
         <v>158</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="1" t="s">
         <v>159</v>
       </c>
@@ -2780,7 +2816,7 @@
         <v>161</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="1" t="s">
         <v>162</v>
       </c>
@@ -2795,7 +2831,7 @@
         <v>164</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="1" t="s">
         <v>165</v>
       </c>
@@ -2810,7 +2846,7 @@
         <v>167</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="1" t="s">
         <v>168</v>
       </c>
@@ -2825,7 +2861,7 @@
         <v>170</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="1" t="s">
         <v>171</v>
       </c>
@@ -2840,7 +2876,7 @@
         <v>173</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="1" t="s">
         <v>174</v>
       </c>
@@ -2855,7 +2891,7 @@
         <v>176</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="1" t="s">
         <v>177</v>
       </c>
@@ -2870,7 +2906,7 @@
         <v>179</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="1" t="s">
         <v>180</v>
       </c>
@@ -2885,7 +2921,7 @@
         <v>182</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="1" t="s">
         <v>183</v>
       </c>
@@ -2900,7 +2936,7 @@
         <v>185</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="1" t="s">
         <v>186</v>
       </c>
@@ -2915,7 +2951,7 @@
         <v>188</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="1" t="s">
         <v>189</v>
       </c>
@@ -2930,7 +2966,7 @@
         <v>191</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="1" t="s">
         <v>192</v>
       </c>
@@ -2945,7 +2981,7 @@
         <v>194</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
       <c r="A62" s="1" t="s">
         <v>195</v>
       </c>
@@ -2960,7 +2996,7 @@
         <v>198</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
       <c r="A63" s="1" t="s">
         <v>199</v>
       </c>
@@ -2975,7 +3011,7 @@
         <v>201</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
       <c r="A64" s="1" t="s">
         <v>202</v>
       </c>
@@ -2990,7 +3026,7 @@
         <v>204</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
       <c r="A65" s="1" t="s">
         <v>205</v>
       </c>
@@ -3005,7 +3041,7 @@
         <v>208</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
       <c r="A66" s="1" t="s">
         <v>209</v>
       </c>
@@ -3020,7 +3056,7 @@
         <v>211</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
       <c r="A67" s="1" t="s">
         <v>212</v>
       </c>
@@ -3035,7 +3071,7 @@
         <v>214</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="1" t="s">
         <v>215</v>
       </c>
@@ -3050,7 +3086,7 @@
         <v>217</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
       <c r="A69" s="1" t="s">
         <v>218</v>
       </c>
@@ -3065,7 +3101,7 @@
         <v>220</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
       <c r="A70" s="1" t="s">
         <v>221</v>
       </c>
@@ -3080,7 +3116,7 @@
         <v>223</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
       <c r="A71" s="1" t="s">
         <v>224</v>
       </c>
@@ -3095,7 +3131,7 @@
         <v>226</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
       <c r="A72" s="1" t="s">
         <v>227</v>
       </c>
@@ -3110,7 +3146,7 @@
         <v>229</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
       <c r="A73" s="1" t="s">
         <v>230</v>
       </c>
@@ -3125,7 +3161,7 @@
         <v>232</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
       <c r="A74" s="1" t="s">
         <v>233</v>
       </c>
@@ -3140,7 +3176,7 @@
         <v>235</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
       <c r="A75" s="1" t="s">
         <v>236</v>
       </c>
@@ -3155,7 +3191,7 @@
         <v>238</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
       <c r="A76" s="1" t="s">
         <v>239</v>
       </c>
@@ -3170,7 +3206,7 @@
         <v>241</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
       <c r="A77" s="1" t="s">
         <v>242</v>
       </c>
@@ -3185,7 +3221,7 @@
         <v>244</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
       <c r="A78" s="1" t="s">
         <v>245</v>
       </c>
@@ -3200,7 +3236,7 @@
         <v>247</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
       <c r="A79" s="1" t="s">
         <v>248</v>
       </c>
@@ -3215,7 +3251,7 @@
         <v>250</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
       <c r="A80" s="1" t="s">
         <v>251</v>
       </c>
@@ -3230,7 +3266,7 @@
         <v>253</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
       <c r="A81" s="1" t="s">
         <v>254</v>
       </c>
@@ -3245,7 +3281,7 @@
         <v>256</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
       <c r="A82" s="1" t="s">
         <v>257</v>
       </c>
@@ -3260,7 +3296,7 @@
         <v>259</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
       <c r="A83" s="1" t="s">
         <v>260</v>
       </c>
@@ -3275,7 +3311,7 @@
         <v>262</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
       <c r="A84" s="1" t="s">
         <v>263</v>
       </c>
@@ -3290,7 +3326,7 @@
         <v>265</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
       <c r="A85" s="1" t="s">
         <v>266</v>
       </c>
@@ -3305,7 +3341,7 @@
         <v>268</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
       <c r="A86" s="1" t="s">
         <v>269</v>
       </c>
@@ -3320,7 +3356,7 @@
         <v>271</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
       <c r="A87" s="1" t="s">
         <v>272</v>
       </c>
@@ -3335,7 +3371,7 @@
         <v>274</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
       <c r="A88" s="1" t="s">
         <v>275</v>
       </c>
@@ -3350,7 +3386,7 @@
         <v>277</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
       <c r="A89" s="1" t="s">
         <v>278</v>
       </c>
@@ -3365,7 +3401,7 @@
         <v>280</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
       <c r="A90" s="1" t="s">
         <v>281</v>
       </c>
@@ -3380,7 +3416,7 @@
         <v>283</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
       <c r="A91" s="1" t="s">
         <v>284</v>
       </c>
@@ -3395,7 +3431,7 @@
         <v>286</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
       <c r="A92" s="1" t="s">
         <v>287</v>
       </c>
@@ -3410,7 +3446,7 @@
         <v>289</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
       <c r="A93" s="1" t="s">
         <v>290</v>
       </c>
@@ -3425,7 +3461,7 @@
         <v>292</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
       <c r="A94" s="1" t="s">
         <v>293</v>
       </c>
@@ -3440,7 +3476,7 @@
         <v>295</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
       <c r="A95" s="1" t="s">
         <v>296</v>
       </c>
@@ -3455,7 +3491,7 @@
         <v>298</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
       <c r="A96" s="1" t="s">
         <v>299</v>
       </c>
@@ -3470,7 +3506,7 @@
         <v>301</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
       <c r="A97" s="1" t="s">
         <v>302</v>
       </c>
@@ -3485,7 +3521,7 @@
         <v>304</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
       <c r="A98" s="1" t="s">
         <v>305</v>
       </c>
@@ -3500,7 +3536,7 @@
         <v>307</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
       <c r="A99" s="1" t="s">
         <v>308</v>
       </c>
@@ -3515,7 +3551,7 @@
         <v>310</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
       <c r="A100" s="1" t="s">
         <v>311</v>
       </c>
@@ -3530,7 +3566,7 @@
         <v>313</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
       <c r="A101" s="1" t="s">
         <v>314</v>
       </c>
@@ -3545,7 +3581,7 @@
         <v>316</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
       <c r="A102" s="1" t="s">
         <v>317</v>
       </c>
@@ -3562,7 +3598,7 @@
         <v>319</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5">
       <c r="A103" s="1" t="s">
         <v>317</v>
       </c>
@@ -3579,7 +3615,7 @@
         <v>320</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
       <c r="A104" s="1" t="s">
         <v>321</v>
       </c>
@@ -3596,7 +3632,7 @@
         <v>324</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5">
       <c r="A105" s="1" t="s">
         <v>325</v>
       </c>
@@ -3613,7 +3649,7 @@
         <v>327</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5">
       <c r="A106" s="1" t="s">
         <v>328</v>
       </c>
@@ -3630,7 +3666,7 @@
         <v>330</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="19.5">
       <c r="A107" s="1" t="s">
         <v>331</v>
       </c>
@@ -3647,7 +3683,7 @@
         <v>333</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="19.5">
       <c r="A108" s="1" t="s">
         <v>334</v>
       </c>
@@ -3664,7 +3700,7 @@
         <v>336</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="19.5">
       <c r="A109" s="1" t="s">
         <v>337</v>
       </c>
@@ -3681,7 +3717,7 @@
         <v>340</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="19.5">
       <c r="A110" s="1" t="s">
         <v>341</v>
       </c>
@@ -3698,7 +3734,7 @@
         <v>343</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="19.5">
       <c r="A111" s="1" t="s">
         <v>344</v>
       </c>
@@ -3715,7 +3751,7 @@
         <v>346</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="19.5">
       <c r="A112" s="1" t="s">
         <v>347</v>
       </c>
@@ -3732,7 +3768,7 @@
         <v>349</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="19.5">
       <c r="A113" s="1" t="s">
         <v>350</v>
       </c>
@@ -3749,7 +3785,7 @@
         <v>352</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="19.5">
       <c r="A114" s="1" t="s">
         <v>353</v>
       </c>
@@ -3766,7 +3802,7 @@
         <v>355</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="19.5">
       <c r="A115" s="1" t="s">
         <v>356</v>
       </c>
@@ -3781,7 +3817,7 @@
         <v>358</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="19.5">
       <c r="A116" s="1" t="s">
         <v>359</v>
       </c>
@@ -3796,7 +3832,7 @@
         <v>361</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="19.5">
       <c r="A117" s="1" t="s">
         <v>362</v>
       </c>
@@ -3811,7 +3847,7 @@
         <v>364</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="19.5">
       <c r="A118" s="1" t="s">
         <v>365</v>
       </c>
@@ -3826,7 +3862,7 @@
         <v>367</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="19.5">
       <c r="A119" s="1" t="s">
         <v>368</v>
       </c>
@@ -3841,7 +3877,7 @@
         <v>370</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="19.5">
       <c r="A120" s="1" t="s">
         <v>371</v>
       </c>
@@ -3856,7 +3892,7 @@
         <v>373</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="19.5">
       <c r="A121" s="1" t="s">
         <v>374</v>
       </c>
@@ -3871,7 +3907,7 @@
         <v>376</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="19.5">
       <c r="A122" s="1" t="s">
         <v>377</v>
       </c>
@@ -3886,7 +3922,7 @@
         <v>379</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="19.5">
       <c r="A123" s="1" t="s">
         <v>380</v>
       </c>
@@ -3901,7 +3937,7 @@
         <v>382</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="19.5">
       <c r="A124" s="1" t="s">
         <v>383</v>
       </c>
@@ -3916,7 +3952,7 @@
         <v>385</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="19.5">
       <c r="A125" s="1" t="s">
         <v>386</v>
       </c>
@@ -3931,7 +3967,7 @@
         <v>388</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="19.5">
       <c r="A126" s="1" t="s">
         <v>389</v>
       </c>
@@ -3946,7 +3982,7 @@
         <v>391</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="19.5">
       <c r="A127" s="1" t="s">
         <v>392</v>
       </c>
@@ -3961,7 +3997,7 @@
         <v>394</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="19.5">
       <c r="A128" s="1" t="s">
         <v>395</v>
       </c>
@@ -3976,7 +4012,7 @@
         <v>398</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="19.5">
       <c r="A129" s="1" t="s">
         <v>399</v>
       </c>
@@ -3991,7 +4027,7 @@
         <v>402</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="19.5">
       <c r="A130" s="1" t="s">
         <v>403</v>
       </c>
@@ -4006,7 +4042,7 @@
         <v>405</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="19.5">
       <c r="A131" s="1" t="s">
         <v>406</v>
       </c>
@@ -4021,7 +4057,7 @@
         <v>408</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="19.5">
       <c r="A132" s="1" t="s">
         <v>409</v>
       </c>
@@ -4036,7 +4072,7 @@
         <v>408</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="19.5">
       <c r="A133" s="1" t="s">
         <v>411</v>
       </c>
@@ -4051,7 +4087,7 @@
         <v>408</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="19.5">
       <c r="A134" s="1" t="s">
         <v>413</v>
       </c>
@@ -4066,7 +4102,7 @@
         <v>408</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="19.5">
       <c r="A135" s="1" t="s">
         <v>415</v>
       </c>
@@ -4081,7 +4117,7 @@
         <v>417</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="19.5">
       <c r="A136" s="1" t="s">
         <v>418</v>
       </c>
@@ -4096,7 +4132,7 @@
         <v>420</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="19.5">
       <c r="A137" s="1" t="s">
         <v>421</v>
       </c>
@@ -4111,7 +4147,7 @@
         <v>420</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="19.5">
       <c r="A138" s="1" t="s">
         <v>423</v>
       </c>
@@ -4126,7 +4162,7 @@
         <v>420</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="19.5">
       <c r="A139" s="1" t="s">
         <v>425</v>
       </c>
@@ -4141,7 +4177,7 @@
         <v>420</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="19.5">
       <c r="A140" s="1" t="s">
         <v>427</v>
       </c>
@@ -4156,7 +4192,7 @@
         <v>429</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="19.5">
       <c r="A141" s="1" t="s">
         <v>430</v>
       </c>
@@ -4171,7 +4207,7 @@
         <v>432</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="19.5">
       <c r="A142" s="1" t="s">
         <v>433</v>
       </c>
@@ -4186,7 +4222,7 @@
         <v>435</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="19.5">
       <c r="A143" s="1" t="s">
         <v>436</v>
       </c>
@@ -4201,7 +4237,7 @@
         <v>438</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="19.5">
       <c r="A144" s="1" t="s">
         <v>439</v>
       </c>
@@ -4216,7 +4252,7 @@
         <v>441</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="19.5">
       <c r="A145" s="1" t="s">
         <v>442</v>
       </c>
@@ -4231,7 +4267,7 @@
         <v>444</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="19.5">
       <c r="A146" s="1" t="s">
         <v>445</v>
       </c>
@@ -4246,7 +4282,7 @@
         <v>447</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="19.5">
       <c r="A147" s="1" t="s">
         <v>448</v>
       </c>
@@ -4261,7 +4297,7 @@
         <v>450</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="19.5">
       <c r="A148" s="1" t="s">
         <v>451</v>
       </c>
@@ -4276,7 +4312,7 @@
         <v>453</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="19.5">
       <c r="A149" s="1" t="s">
         <v>454</v>
       </c>
@@ -4291,7 +4327,7 @@
         <v>456</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="19.5">
       <c r="A150" s="1" t="s">
         <v>457</v>
       </c>
@@ -4306,7 +4342,7 @@
         <v>460</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="19.5">
       <c r="A151" s="1" t="s">
         <v>461</v>
       </c>
@@ -4321,7 +4357,7 @@
         <v>463</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="19.5">
       <c r="A152" s="1" t="s">
         <v>464</v>
       </c>
@@ -4336,7 +4372,7 @@
         <v>466</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="19.5">
       <c r="A153" s="1" t="s">
         <v>467</v>
       </c>
@@ -4351,7 +4387,7 @@
         <v>470</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
       <c r="A154" s="1" t="s">
         <v>471</v>
       </c>
@@ -4363,25 +4399,25 @@
         <v>469</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="19.5" hidden="1">
+        <v>473</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="19.5">
       <c r="A155" s="1" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B155" s="1"/>
       <c r="C155" s="1" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>469</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="19.5" hidden="1">
+        <v>470</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="19.5">
       <c r="A156" s="1" t="s">
         <v>476</v>
       </c>
@@ -4396,7 +4432,7 @@
         <v>478</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="19.5">
       <c r="A157" s="1" t="s">
         <v>479</v>
       </c>
@@ -4408,16 +4444,16 @@
         <v>469</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="19.5" hidden="1">
+        <v>481</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="19.5">
       <c r="A158" s="1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B158" s="1"/>
       <c r="C158" s="1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>469</v>
@@ -4426,22 +4462,22 @@
         <v>470</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="19.5">
       <c r="A159" s="1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B159" s="1"/>
       <c r="C159" s="1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>469</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5" hidden="1">
+        <v>470</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5">
       <c r="A160" s="1" t="s">
         <v>486</v>
       </c>
@@ -4456,7 +4492,7 @@
         <v>488</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="19.5">
       <c r="A161" s="1" t="s">
         <v>489</v>
       </c>
@@ -4471,7 +4507,7 @@
         <v>491</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="19.5">
       <c r="A162" s="1" t="s">
         <v>492</v>
       </c>
@@ -4486,7 +4522,7 @@
         <v>494</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
       <c r="A163" s="1" t="s">
         <v>495</v>
       </c>
@@ -4501,7 +4537,7 @@
         <v>497</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="19.5">
       <c r="A164" s="1" t="s">
         <v>498</v>
       </c>
@@ -4510,13 +4546,13 @@
         <v>499</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>49</v>
+        <v>469</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
       <c r="A165" s="1" t="s">
         <v>501</v>
       </c>
@@ -4525,13 +4561,13 @@
         <v>502</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>49</v>
+        <v>469</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>503</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="19.5">
       <c r="A166" s="1" t="s">
         <v>504</v>
       </c>
@@ -4540,13 +4576,13 @@
         <v>505</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>106</v>
+        <v>469</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>506</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
       <c r="A167" s="1" t="s">
         <v>507</v>
       </c>
@@ -4555,7 +4591,7 @@
         <v>508</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>106</v>
+        <v>469</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>509</v>
@@ -4576,7 +4612,7 @@
         <v>512</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="19.5">
       <c r="A169" s="1" t="s">
         <v>513</v>
       </c>
@@ -4591,7 +4627,7 @@
         <v>515</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="19.5">
       <c r="A170" s="1" t="s">
         <v>516</v>
       </c>
@@ -4600,13 +4636,13 @@
         <v>517</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>518</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="19.5">
       <c r="A171" s="1" t="s">
         <v>519</v>
       </c>
@@ -4615,13 +4651,13 @@
         <v>520</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>521</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="19.5">
       <c r="A172" s="1" t="s">
         <v>522</v>
       </c>
@@ -4630,73 +4666,73 @@
         <v>523</v>
       </c>
       <c r="D172" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E172" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="E172" s="1" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
+      <c r="A173" s="1" t="s">
         <v>525</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="19.5" hidden="1">
-      <c r="A173" s="1" t="s">
-        <v>526</v>
       </c>
       <c r="B173" s="1"/>
       <c r="C173" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E173" s="1" t="s">
         <v>527</v>
       </c>
-      <c r="D173" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="E173" s="1" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75" hidden="1">
+      <c r="A174" s="1" t="s">
         <v>528</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="19.5" hidden="1">
-      <c r="A174" s="1" t="s">
-        <v>529</v>
       </c>
       <c r="B174" s="1"/>
       <c r="C174" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E174" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="D174" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E174" s="1" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75" hidden="1">
+      <c r="A175" s="1" t="s">
         <v>531</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="19.5" hidden="1">
-      <c r="A175" s="1" t="s">
-        <v>532</v>
       </c>
       <c r="B175" s="1"/>
       <c r="C175" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E175" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="D175" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E175" s="1" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75" hidden="1">
+      <c r="A176" s="1" t="s">
         <v>534</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="19.5" hidden="1">
-      <c r="A176" s="1" t="s">
-        <v>535</v>
       </c>
       <c r="B176" s="1"/>
       <c r="C176" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D176" s="1" t="s">
         <v>536</v>
-      </c>
-      <c r="D176" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>537</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="19.5" hidden="1">
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75" hidden="1">
       <c r="A177" s="1" t="s">
         <v>538</v>
       </c>
@@ -4709,6 +4745,66 @@
       </c>
       <c r="E177" s="1" t="s">
         <v>540</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75" hidden="1">
+      <c r="A178" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="B178" s="1"/>
+      <c r="C178" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75" hidden="1">
+      <c r="A179" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B179" s="1"/>
+      <c r="C179" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75" hidden="1">
+      <c r="A180" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="B180" s="1"/>
+      <c r="C180" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75" hidden="1">
+      <c r="A181" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="B181" s="1"/>
+      <c r="C181" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OE-9291 - Make descripton and group required
</commit_message>
<xml_diff>
--- a/protected/migrations/data/m221109_114900_add_description_grouping_to_settings/setting_metadata_202208211803.xlsx
+++ b/protected/migrations/data/m221109_114900_add_description_grouping_to_settings/setting_metadata_202208211803.xlsx
@@ -163,16 +163,16 @@
     <t>Auto-complete text inputs</t>
   </si>
   <si>
+    <t>(NEEDS REMOVING) In old browsers, this used to determine if the browser&amp;apos;s "Auto Complete" function for text fields was enabled or not. Moden browsers tend to ignore this and apply their own rules</t>
+  </si>
+  <si>
+    <t>watermark</t>
+  </si>
+  <si>
+    <t>User Banner</t>
+  </si>
+  <si>
     <t>Core</t>
-  </si>
-  <si>
-    <t>(NEEDS REMOVING) In old browsers, this used to determine if the browser&amp;apos;s "Auto Complete" function for text fields was enabled or not. Moden browsers tend to ignore this and apply their own rules</t>
-  </si>
-  <si>
-    <t>watermark</t>
-  </si>
-  <si>
-    <t>User Banner</t>
   </si>
   <si>
     <t>The long version of the banner that will be shown on all pages of the site TO ORDINARY USERS (in the bottom right for the standard desktop view). This usually displays in full on the login page, but users will need to hover over the banner to dispplay this long message. Also see "User Banner Short" setting</t>
@@ -1463,7 +1463,7 @@
     <t>CVI delivery to LA: Body</t>
   </si>
   <si>
-    <t>The body text for emails sent to Local Authorities for Certificae of Visual Impairment applications. Note that the actual application is attached to the email as a PDF</t>
+    <t>The body text for emails sent to Local Authorities for Certificate of Visual Impairment applications. Note that the actual application is attached to the email as a PDF</t>
   </si>
   <si>
     <t>cvidelivery_rcop_sender_email</t>
@@ -1640,7 +1640,7 @@
     <t>Require PIN for CVI signing</t>
   </si>
   <si>
-    <t>When On, users must sign CVI events using their PINl. When Off, CVI events will be automatically signed for the current user on save</t>
+    <t>When On, users must sign CVI events using their PIN. When Off, CVI events will be automatically signed for the current user on save</t>
   </si>
   <si>
     <t>close_incomplete_exam_elements</t>
@@ -2283,22 +2283,22 @@
         <v>48</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>53</v>
@@ -2313,7 +2313,7 @@
         <v>55</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>56</v>
@@ -2328,7 +2328,7 @@
         <v>58</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>59</v>
@@ -2343,7 +2343,7 @@
         <v>61</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>62</v>
@@ -2358,7 +2358,7 @@
         <v>64</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>65</v>
@@ -2373,7 +2373,7 @@
         <v>67</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>68</v>
@@ -2480,7 +2480,7 @@
         <v>92</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>93</v>
@@ -2600,7 +2600,7 @@
         <v>118</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>119</v>
@@ -2615,7 +2615,7 @@
         <v>121</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>122</v>
@@ -2660,7 +2660,7 @@
         <v>130</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>131</v>
@@ -2705,7 +2705,7 @@
         <v>139</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>140</v>
@@ -2720,7 +2720,7 @@
         <v>142</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>143</v>
@@ -2765,7 +2765,7 @@
         <v>151</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>152</v>
@@ -2810,7 +2810,7 @@
         <v>160</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>161</v>
@@ -2855,7 +2855,7 @@
         <v>169</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>170</v>
@@ -2870,7 +2870,7 @@
         <v>172</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>173</v>
@@ -2885,7 +2885,7 @@
         <v>175</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>176</v>
@@ -2900,7 +2900,7 @@
         <v>178</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>179</v>
@@ -2915,7 +2915,7 @@
         <v>181</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>182</v>
@@ -2930,7 +2930,7 @@
         <v>184</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>185</v>
@@ -2945,7 +2945,7 @@
         <v>187</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>188</v>
@@ -2960,7 +2960,7 @@
         <v>190</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>191</v>
@@ -2975,7 +2975,7 @@
         <v>193</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>194</v>
@@ -3185,7 +3185,7 @@
         <v>237</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>238</v>
@@ -3200,7 +3200,7 @@
         <v>240</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>241</v>
@@ -3290,7 +3290,7 @@
         <v>258</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>259</v>
@@ -3305,7 +3305,7 @@
         <v>261</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>262</v>
@@ -3320,7 +3320,7 @@
         <v>264</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>265</v>
@@ -3335,7 +3335,7 @@
         <v>267</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>268</v>
@@ -3395,7 +3395,7 @@
         <v>279</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>280</v>
@@ -3410,7 +3410,7 @@
         <v>282</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>283</v>
@@ -3425,7 +3425,7 @@
         <v>285</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>286</v>
@@ -3455,7 +3455,7 @@
         <v>291</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>292</v>
@@ -3470,7 +3470,7 @@
         <v>294</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>295</v>
@@ -3545,7 +3545,7 @@
         <v>309</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>310</v>
@@ -3575,7 +3575,7 @@
         <v>315</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>316</v>
@@ -3811,7 +3811,7 @@
         <v>357</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>358</v>
@@ -3826,7 +3826,7 @@
         <v>360</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>361</v>
@@ -3841,7 +3841,7 @@
         <v>363</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>364</v>
@@ -3856,7 +3856,7 @@
         <v>366</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>367</v>
@@ -3871,7 +3871,7 @@
         <v>369</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>370</v>
@@ -3886,7 +3886,7 @@
         <v>372</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>373</v>
@@ -3901,7 +3901,7 @@
         <v>375</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>376</v>
@@ -3961,7 +3961,7 @@
         <v>387</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>388</v>
@@ -4036,7 +4036,7 @@
         <v>404</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>405</v>
@@ -4051,7 +4051,7 @@
         <v>407</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>408</v>
@@ -4066,7 +4066,7 @@
         <v>410</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>408</v>
@@ -4081,7 +4081,7 @@
         <v>412</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>408</v>
@@ -4096,7 +4096,7 @@
         <v>414</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>408</v>
@@ -4111,7 +4111,7 @@
         <v>416</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>417</v>
@@ -4126,7 +4126,7 @@
         <v>419</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>420</v>
@@ -4141,7 +4141,7 @@
         <v>422</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>420</v>
@@ -4156,7 +4156,7 @@
         <v>424</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>420</v>
@@ -4171,7 +4171,7 @@
         <v>426</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>420</v>
@@ -4186,7 +4186,7 @@
         <v>428</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>429</v>
@@ -4261,7 +4261,7 @@
         <v>443</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>444</v>
@@ -4606,7 +4606,7 @@
         <v>511</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>512</v>
@@ -4621,7 +4621,7 @@
         <v>514</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>515</v>
@@ -4666,7 +4666,7 @@
         <v>523</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>49</v>
+        <v>13</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>524</v>
@@ -4681,13 +4681,13 @@
         <v>526</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>527</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
       <c r="A174" s="1" t="s">
         <v>528</v>
       </c>
@@ -4702,7 +4702,7 @@
         <v>530</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
       <c r="A175" s="1" t="s">
         <v>531</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>533</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
       <c r="A176" s="1" t="s">
         <v>534</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>537</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
       <c r="A177" s="1" t="s">
         <v>538</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>540</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
       <c r="A178" s="1" t="s">
         <v>541</v>
       </c>
@@ -4762,7 +4762,7 @@
         <v>543</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
       <c r="A179" s="1" t="s">
         <v>544</v>
       </c>
@@ -4771,13 +4771,13 @@
         <v>545</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>546</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
       <c r="A180" s="1" t="s">
         <v>547</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>549</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75" hidden="1">
+    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="19.5">
       <c r="A181" s="1" t="s">
         <v>550</v>
       </c>

</xml_diff>